<commit_message>
added na removal and toc
</commit_message>
<xml_diff>
--- a/Planning-Overview-Presentation.xlsx
+++ b/Planning-Overview-Presentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adyan.rios\Documents\GitHub\SEFSC\SEFSC-Caribbean-Strategic-Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82B4400-60F9-463D-8BFA-772499A7141F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F821D04B-F581-4162-8588-F100EED34DC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning-Overview-Presentation" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>organizations</t>
   </si>
   <si>
-    <t>start_year</t>
-  </si>
-  <si>
     <t>PR, USVI</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Strategic Planning</t>
   </si>
   <si>
-    <t>lead_program</t>
-  </si>
-  <si>
     <t>Create a portfolio (slide deck) of who we are and what projects we work on</t>
   </si>
   <si>
@@ -128,15 +122,6 @@
     <t>Kim Johnson</t>
   </si>
   <si>
-    <t>target_species</t>
-  </si>
-  <si>
-    <t>depth_range</t>
-  </si>
-  <si>
-    <t>end_year</t>
-  </si>
-  <si>
     <t>images</t>
   </si>
   <si>
@@ -455,9 +440,6 @@
     <t>Planned</t>
   </si>
   <si>
-    <t>poc_website</t>
-  </si>
-  <si>
     <t>https://www.fisheries.noaa.gov/contact/steven-g-smith-phd</t>
   </si>
   <si>
@@ -498,6 +480,24 @@
   </si>
   <si>
     <t>https://dpnr.vi.gov/fish-and-wildlife/</t>
+  </si>
+  <si>
+    <t>lead program</t>
+  </si>
+  <si>
+    <t>target species</t>
+  </si>
+  <si>
+    <t>depth range</t>
+  </si>
+  <si>
+    <t>start year</t>
+  </si>
+  <si>
+    <t>end year</t>
+  </si>
+  <si>
+    <t>website</t>
   </si>
 </sst>
 </file>
@@ -1358,53 +1358,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="6" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.21875" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
         <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -1416,1052 +1415,1052 @@
         <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
       <c r="M1" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
       <c r="O1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>157</v>
+      </c>
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P2">
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P3">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>39</v>
-      </c>
       <c r="O4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P4">
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P5">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P6">
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="O7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P7">
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P8">
         <v>2023</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P9">
         <v>2023</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="O10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P10">
         <v>2023</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P11">
         <v>2023</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O12" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P12">
         <v>2023</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P13">
         <v>2023</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="O14" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P14">
         <v>2023</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" t="s">
         <v>74</v>
       </c>
-      <c r="F15" t="s">
+      <c r="K15" t="s">
         <v>75</v>
       </c>
-      <c r="G15" t="s">
+      <c r="N15" t="s">
         <v>76</v>
       </c>
-      <c r="H15" t="s">
-        <v>77</v>
-      </c>
-      <c r="I15" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" t="s">
-        <v>80</v>
-      </c>
-      <c r="N15" t="s">
-        <v>81</v>
-      </c>
       <c r="O15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P15">
         <v>2021</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" t="s">
         <v>79</v>
       </c>
-      <c r="K16" t="s">
-        <v>84</v>
-      </c>
       <c r="N16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="O16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P16">
         <v>1983</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" t="s">
         <v>83</v>
       </c>
-      <c r="J17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K17" t="s">
-        <v>88</v>
-      </c>
       <c r="N17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="O17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P17">
         <v>1974</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18" t="s">
         <v>79</v>
       </c>
-      <c r="K18" t="s">
-        <v>84</v>
-      </c>
       <c r="N18" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P18">
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" t="s">
         <v>83</v>
       </c>
-      <c r="J19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="N19" t="s">
         <v>88</v>
       </c>
-      <c r="N19" t="s">
-        <v>93</v>
-      </c>
       <c r="O19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P19">
         <v>2016</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="O20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P20">
         <v>2022</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
+        <v>74</v>
+      </c>
+      <c r="K21" t="s">
         <v>79</v>
       </c>
-      <c r="K21" t="s">
-        <v>84</v>
-      </c>
       <c r="N21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O21" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P21">
         <v>1983</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" t="s">
+        <v>82</v>
+      </c>
+      <c r="K22" t="s">
         <v>83</v>
       </c>
-      <c r="J22" t="s">
-        <v>87</v>
-      </c>
-      <c r="K22" t="s">
-        <v>88</v>
-      </c>
       <c r="N22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O22" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P22">
         <v>1979</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J23" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" t="s">
         <v>79</v>
       </c>
-      <c r="K23" t="s">
-        <v>84</v>
-      </c>
       <c r="N23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="O23" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P23">
         <v>2022</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N24" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="O24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P24">
         <v>2012</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" t="s">
+        <v>99</v>
+      </c>
+      <c r="M25" t="s">
         <v>103</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>104</v>
       </c>
-      <c r="M25" t="s">
-        <v>108</v>
-      </c>
-      <c r="N25" t="s">
-        <v>109</v>
-      </c>
       <c r="O25" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P25">
         <v>2016</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="N26" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="O26" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P26">
         <v>2016</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L27" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M27" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O27" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P27">
         <v>2022</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="L28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N28" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="O28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N29" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="O29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P29">
         <v>2022</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F30" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I30" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="L30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N30" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="O30" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P30">
         <v>2020</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I31" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N31" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O31" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P31">
         <v>2020</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H32" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L32" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N32" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="O32" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P32">
         <v>2021</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O33" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P33">
         <v>2022</v>
@@ -2470,33 +2469,33 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O34" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P34">
         <v>2022</v>
@@ -2505,33 +2504,33 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O35" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P35">
         <v>2022</v>
@@ -2540,33 +2539,33 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F36" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" t="s">
-        <v>23</v>
-      </c>
       <c r="O36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P36">
         <v>2022</v>
@@ -2575,33 +2574,33 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F37" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" t="s">
-        <v>23</v>
-      </c>
       <c r="O37" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P37">
         <v>2023</v>
@@ -2610,120 +2609,120 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G38" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H38" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J38" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K38" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N38" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="O38" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P38">
         <v>2024</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G39" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H39" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I39" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J39" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K39" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N39" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="O39" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P39">
         <v>2025</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>129</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" t="s">
+        <v>98</v>
+      </c>
+      <c r="L40" t="s">
+        <v>108</v>
+      </c>
+      <c r="M40" t="s">
+        <v>130</v>
+      </c>
+      <c r="N40" t="s">
+        <v>131</v>
+      </c>
+      <c r="O40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" t="s">
+        <v>71</v>
+      </c>
+      <c r="H41" t="s">
+        <v>98</v>
+      </c>
+      <c r="L41" t="s">
+        <v>133</v>
+      </c>
+      <c r="M41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N41" t="s">
         <v>134</v>
       </c>
-      <c r="F40" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" t="s">
-        <v>76</v>
-      </c>
-      <c r="H40" t="s">
-        <v>103</v>
-      </c>
-      <c r="L40" t="s">
-        <v>113</v>
-      </c>
-      <c r="M40" t="s">
-        <v>135</v>
-      </c>
-      <c r="N40" t="s">
-        <v>136</v>
-      </c>
-      <c r="O40" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" t="s">
-        <v>76</v>
-      </c>
-      <c r="H41" t="s">
-        <v>103</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="O41" t="s">
         <v>138</v>
-      </c>
-      <c r="M41" t="s">
-        <v>135</v>
-      </c>
-      <c r="N41" t="s">
-        <v>139</v>
-      </c>
-      <c r="O41" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2758,7 +2757,7 @@
       <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>